<commit_message>
Add url for february forecast errors.
</commit_message>
<xml_diff>
--- a/FebuaryForecastErrors/FebruaryForecastErrors.xlsx
+++ b/FebuaryForecastErrors/FebruaryForecastErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\FebuaryForecastErrors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF9C9E-96A5-435F-A047-7DAA794D0AE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901E231-6ECF-4498-940B-F9B85F295072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7670" xr2:uid="{C4AE9992-B04D-48E7-BF40-062161DCF152}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{C4AE9992-B04D-48E7-BF40-062161DCF152}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Feb. 1 forecast</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>https://www.inkstain.net/2023/02/deadpool-diaries-ignore-this-post-about-the-latest-colorado-river-runoff-forecast/</t>
   </si>
 </sst>
 </file>
@@ -136,9 +139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -176,7 +179,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -282,7 +285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,7 +427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DB4E93-160D-4514-9B0E-03E303766D71}">
-  <dimension ref="A3:D19"/>
+  <dimension ref="A3:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,213 +456,221 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9000</v>
-      </c>
-      <c r="C6" s="2">
-        <v>11500</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5050</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1910</v>
-      </c>
-      <c r="D7" s="2">
-        <v>-3140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B8" s="2">
-        <v>3850</v>
+        <v>9000</v>
       </c>
       <c r="C8" s="2">
-        <v>2560</v>
+        <v>11500</v>
       </c>
       <c r="D8" s="2">
-        <v>-1290</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B9" s="2">
-        <v>7250</v>
+        <v>5050</v>
       </c>
       <c r="C9" s="2">
-        <v>6920</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-330</v>
+        <v>1910</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-3140</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B10" s="2">
-        <v>5200</v>
+        <v>3850</v>
       </c>
       <c r="C10" s="2">
-        <v>6710</v>
+        <v>2560</v>
       </c>
       <c r="D10" s="2">
-        <v>1510</v>
+        <v>-1290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B11" s="2">
-        <v>6400</v>
+        <v>7250</v>
       </c>
       <c r="C11" s="2">
-        <v>6630</v>
+        <v>6920</v>
       </c>
       <c r="D11" s="1">
-        <v>230</v>
+        <v>-330</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B12" s="2">
-        <v>9600</v>
+        <v>5200</v>
       </c>
       <c r="C12" s="2">
-        <v>8170</v>
+        <v>6710</v>
       </c>
       <c r="D12" s="2">
-        <v>-1430</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B13" s="2">
-        <v>3900</v>
+        <v>6400</v>
       </c>
       <c r="C13" s="2">
-        <v>2600</v>
-      </c>
-      <c r="D13" s="2">
-        <v>-1300</v>
+        <v>6630</v>
+      </c>
+      <c r="D13" s="1">
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B14" s="2">
-        <v>5300</v>
+        <v>9600</v>
       </c>
       <c r="C14" s="2">
-        <v>10400</v>
+        <v>8170</v>
       </c>
       <c r="D14" s="2">
-        <v>5100</v>
+        <v>-1430</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="B15" s="2">
-        <v>5700</v>
+        <v>3900</v>
       </c>
       <c r="C15" s="2">
-        <v>3760</v>
+        <v>2600</v>
       </c>
       <c r="D15" s="2">
-        <v>-1940</v>
+        <v>-1300</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B16" s="2">
-        <v>3300</v>
+        <v>5300</v>
       </c>
       <c r="C16" s="2">
-        <v>1850</v>
+        <v>10400</v>
       </c>
       <c r="D16" s="2">
-        <v>-1450</v>
+        <v>5100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5700</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3760</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-1940</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3300</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1850</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-1450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>2022</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B19" s="2">
         <v>5000</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C19" s="2">
         <v>3750</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D19" s="2">
         <v>-1250</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B20" s="2">
         <v>5796</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C20" s="2">
         <v>5563</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D20" s="1">
         <v>-233</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B21" s="2">
         <v>5250</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C21" s="2">
         <v>5195</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>-1270</v>
       </c>
     </row>

</xml_diff>